<commit_message>
Shipment Module-> Manual Shipment Creation and Manual Payment Creation
</commit_message>
<xml_diff>
--- a/AportalRefactor/AportalRefactor/src/main/java/Utilities/Items.xlsx
+++ b/AportalRefactor/AportalRefactor/src/main/java/Utilities/Items.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="9795" activeTab="1"/>
+    <workbookView windowWidth="24000" windowHeight="9795" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Item Name</t>
   </si>
@@ -81,6 +83,33 @@
   </si>
   <si>
     <t>via BestBuy</t>
+  </si>
+  <si>
+    <t>Tracking Number</t>
+  </si>
+  <si>
+    <t>Sender Email</t>
+  </si>
+  <si>
+    <t>KH Notes</t>
+  </si>
+  <si>
+    <t>TBA215215215212</t>
+  </si>
+  <si>
+    <t>farhanahmed.projectmarker@gmail.com</t>
+  </si>
+  <si>
+    <t>Test KH Notes</t>
+  </si>
+  <si>
+    <t>User Email</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>TBA300300300306</t>
   </si>
 </sst>
 </file>
@@ -89,9 +118,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -127,6 +156,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -134,6 +171,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -143,29 +195,38 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,17 +240,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,68 +270,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,37 +314,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,145 +482,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,6 +519,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,6 +567,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -529,15 +587,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -571,171 +620,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -745,8 +774,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,7 +1054,7 @@
     <col min="7" max="7" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="12.75" spans="1:7">
+    <row r="1" s="6" customFormat="1" ht="12.75" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1096,7 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1085,8 +1114,8 @@
   <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1143,4 +1172,102 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="47.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="46.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" ht="14.25" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="farhanahmed.projectmarker@gmail.com" tooltip="mailto:farhanahmed.projectmarker@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="47.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" ht="14.25" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="farhanahmed.projectmarker@gmail.com" tooltip="mailto:farhanahmed.projectmarker@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>